<commit_message>
doc updated for UC#100
</commit_message>
<xml_diff>
--- a/doc/_Requrements.xlsx
+++ b/doc/_Requrements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\github\vadim-kosarev\fc\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9000379A-8B2A-408B-8849-BE0163283DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84540151-497E-41B8-9F28-0ABC0C39FC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="760" windowWidth="27590" windowHeight="15950" xr2:uid="{9180FCDB-912B-4427-B61B-DDCE8FA014C3}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="_ListValues" sheetId="3" r:id="rId2"/>
     <sheet name="100-x-image-input" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">_Main!$A$1:$G$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,15 +39,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>Use Case #</t>
   </si>
   <si>
     <t>Use Case Summary</t>
-  </si>
-  <si>
-    <t>I need to format and encode a message with image within to put it into MQ for further processing</t>
   </si>
   <si>
     <t>Use Case Details</t>
@@ -184,6 +184,45 @@
   </si>
   <si>
     <t>DOC DEVELOPMENT</t>
+  </si>
+  <si>
+    <t>UC#100 should work with Host Web Camera in Laptop  All data (timestamps, ids, frameNo-s etc…) should be calculated correctly</t>
+  </si>
+  <si>
+    <t>The system should be configurable to switch between RabbitMQ and Kafka MQ brokers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python code is configured in fc.python\app-config.ini
+Java code is configured in &lt;TBD&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I need to format and encode a message with single image within to put it into MQ for further processing
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC#100 should work with web camera from Camo Studio (using smartphone) for 4K and 2K videos.  All data (timestamps, ids, frameNo-s etc…) should be calculated correctly
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC#100 should work with recorded static VideoFile. All data (timestamps, ids, frameNo-s etc…) should be calculated correctly
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC#100 should work with Youttube video live stream. All data (timestamps, ids, frameNo-s etc…) should be calculated correctly
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC#100 should work with RTSP-stream. All data (timestamps, ids, frameNo-s etc…) should be calculated correctly
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applications should provide versioin info (major, minor, build, git-hash)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system should provide prometheus data for collecting on dashboard
+</t>
   </si>
 </sst>
 </file>
@@ -296,32 +335,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -649,15 +667,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BEA9E3B-8BD1-4D8E-944C-97151E480D21}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10"/>
   <cols>
-    <col min="1" max="3" width="14.81640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="11.08984375" style="2" customWidth="1"/>
     <col min="4" max="4" width="44.36328125" style="3" customWidth="1"/>
     <col min="5" max="5" width="48.1796875" style="2" customWidth="1"/>
     <col min="6" max="6" width="45.90625" style="2" customWidth="1"/>
@@ -670,65 +689,170 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="30">
+      <c r="A2" s="2">
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30">
+      <c r="A3" s="2">
+        <v>100</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="20">
-      <c r="A2" s="2">
-        <v>100</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="30">
       <c r="A4" s="2">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>101</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="40">
       <c r="A5" s="2">
-        <v>400</v>
+        <v>102</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30">
+      <c r="A6" s="2">
+        <v>103</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30">
+      <c r="A7" s="2">
+        <v>104</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30">
+      <c r="A8" s="2">
+        <v>105</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30">
+      <c r="A9" s="2">
+        <v>150</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30">
+      <c r="A10" s="2">
+        <v>170</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G1" xr:uid="{9BEA9E3B-8BD1-4D8E-944C-97151E480D21}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G10">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"IMPLEMENTED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"OPEN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -782,27 +906,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -830,139 +954,139 @@
   <sheetData>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="10.5">
       <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>16</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="6">
         <v>79</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="6">
         <v>382991</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="6">
         <v>1712372019</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="6">
         <v>1712372023</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="10.5">
       <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="C15" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="230">
       <c r="B16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added java-module for command line client
</commit_message>
<xml_diff>
--- a/doc/_Requrements.xlsx
+++ b/doc/_Requrements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\github\vadim-kosarev\fc\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84540151-497E-41B8-9F28-0ABC0C39FC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E30A44-2D00-44BC-B59D-1DCD57E10E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="27590" windowHeight="15950" xr2:uid="{9180FCDB-912B-4427-B61B-DDCE8FA014C3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="37010" windowHeight="21820" xr2:uid="{9180FCDB-912B-4427-B61B-DDCE8FA014C3}"/>
   </bookViews>
   <sheets>
     <sheet name="_Main" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t>Use Case #</t>
   </si>
@@ -223,6 +223,10 @@
   <si>
     <t xml:space="preserve">The system should provide prometheus data for collecting on dashboard
 </t>
+  </si>
+  <si>
+    <t>gradlew :modules:apps-data-publisher:assemble
+java -jar ./modules/apps-data-publisher/build/libs/apps-data-publisher-0.0.1-SNAPSHOT.jar --file=data/orban_putin.jpg</t>
   </si>
 </sst>
 </file>
@@ -670,7 +674,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10"/>
@@ -679,8 +683,8 @@
     <col min="2" max="3" width="11.08984375" style="2" customWidth="1"/>
     <col min="4" max="4" width="44.36328125" style="3" customWidth="1"/>
     <col min="5" max="5" width="48.1796875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="45.90625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.36328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="46.54296875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="48.453125" style="2" customWidth="1"/>
     <col min="8" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
@@ -724,7 +728,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30">
+    <row r="3" spans="1:7" ht="40">
       <c r="A3" s="2">
         <v>100</v>
       </c>
@@ -743,8 +747,11 @@
       <c r="F3" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="30">
+      <c r="G3" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20">
       <c r="A4" s="2">
         <v>101</v>
       </c>

</xml_diff>

<commit_message>
added frameStoragePath to spec. todo: implement
</commit_message>
<xml_diff>
--- a/doc/_Requrements.xlsx
+++ b/doc/_Requrements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\github\vadim-kosarev\fc\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E30A44-2D00-44BC-B59D-1DCD57E10E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC893998-B8EE-4C88-8253-2004086FF739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="37010" windowHeight="21820" xr2:uid="{9180FCDB-912B-4427-B61B-DDCE8FA014C3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="21648" windowHeight="13176" activeTab="2" xr2:uid="{9180FCDB-912B-4427-B61B-DDCE8FA014C3}"/>
   </bookViews>
   <sheets>
     <sheet name="_Main" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
   <si>
     <t>Use Case #</t>
   </si>
@@ -227,6 +227,23 @@
   <si>
     <t>gradlew :modules:apps-data-publisher:assemble
 java -jar ./modules/apps-data-publisher/build/libs/apps-data-publisher-0.0.1-SNAPSHOT.jar --file=data/orban_putin.jpg</t>
+  </si>
+  <si>
+    <t>Processed image must be saved to Minio at identifier, described on 100-x-image-input</t>
+  </si>
+  <si>
+    <t>frameStoragePath</t>
+  </si>
+  <si>
+    <t>local/jpgdata/{hostname}/{source}/frame_{timestamp}_{frameNo}_{localID}.jpg
+Replacement map:
+":": "_#_",
+"\": "/",
+"//": "/",</t>
+  </si>
+  <si>
+    <t>local/jpgdata/HARON/Camera_#_0/frame_1712372019_15_382991.jpg
+local/jpgdata/HARON/C_#_/dev/github/fc/data/video.avi/frame_1712372019_15_382991.jpg</t>
   </si>
 </sst>
 </file>
@@ -350,14 +367,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -671,24 +688,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BEA9E3B-8BD1-4D8E-944C-97151E480D21}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="11.08984375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="44.36328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="48.1796875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="46.54296875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="48.453125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="14.77734375" style="2" customWidth="1"/>
+    <col min="2" max="3" width="11.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="48.21875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="46.5546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="48.44140625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="10.5">
+    <row r="1" spans="1:7" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -711,7 +728,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30">
+    <row r="2" spans="1:7" ht="30.6">
       <c r="A2" s="2">
         <v>50</v>
       </c>
@@ -728,7 +745,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="40">
+    <row r="3" spans="1:7" ht="40.799999999999997">
       <c r="A3" s="2">
         <v>100</v>
       </c>
@@ -751,7 +768,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="20">
+    <row r="4" spans="1:7" ht="20.399999999999999">
       <c r="A4" s="2">
         <v>101</v>
       </c>
@@ -765,7 +782,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="40">
+    <row r="5" spans="1:7" ht="40.799999999999997">
       <c r="A5" s="2">
         <v>102</v>
       </c>
@@ -779,7 +796,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="30.6">
       <c r="A6" s="2">
         <v>103</v>
       </c>
@@ -793,7 +810,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30">
+    <row r="7" spans="1:7" ht="30.6">
       <c r="A7" s="2">
         <v>104</v>
       </c>
@@ -807,7 +824,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30">
+    <row r="8" spans="1:7" ht="30.6">
       <c r="A8" s="2">
         <v>105</v>
       </c>
@@ -821,7 +838,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
+    <row r="9" spans="1:7" ht="30.6">
       <c r="A9" s="2">
         <v>150</v>
       </c>
@@ -835,7 +852,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30">
+    <row r="10" spans="1:7" ht="30.6">
       <c r="A10" s="2">
         <v>170</v>
       </c>
@@ -847,6 +864,20 @@
       </c>
       <c r="D10" s="3" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20.399999999999999">
+      <c r="A11" s="2">
+        <v>200</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -856,11 +887,11 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"OPEN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"IMPLEMENTED"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"OPEN"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -905,13 +936,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="11.4"/>
   <cols>
-    <col min="1" max="1" width="24.81640625" style="10" customWidth="1"/>
-    <col min="2" max="16384" width="8.7265625" style="10"/>
+    <col min="1" max="1" width="24.77734375" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="8.77734375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" ht="12">
       <c r="A1" s="9" t="s">
         <v>38</v>
       </c>
@@ -944,19 +975,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7EA22A1-2400-4FDB-B83E-AF4FE80BE34F}">
-  <dimension ref="A2:D16"/>
+  <dimension ref="A2:D17"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999"/>
   <cols>
-    <col min="1" max="1" width="29.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.90625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="28.81640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="90.1796875" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="29.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="90.21875" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
@@ -991,7 +1022,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="10.5">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1071,32 +1102,44 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="10.5">
-      <c r="A15" s="1" t="s">
+    <row r="14" spans="1:4" ht="61.2">
+      <c r="B14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="230">
-      <c r="B16" s="6" t="s">
+    <row r="17" spans="2:4" ht="234.6">
+      <c r="B17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C17" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D17" s="8" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Extracted structures into separated model, json serialization of faceBoxes, format for output of detections in python
</commit_message>
<xml_diff>
--- a/doc/_Requrements.xlsx
+++ b/doc/_Requrements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\github\vadim-kosarev\fc\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC893998-B8EE-4C88-8253-2004086FF739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8FA067-BEC5-4E82-948E-52CCF4F94AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21648" windowHeight="13176" activeTab="2" xr2:uid="{9180FCDB-912B-4427-B61B-DDCE8FA014C3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="37010" windowHeight="21820" xr2:uid="{9180FCDB-912B-4427-B61B-DDCE8FA014C3}"/>
   </bookViews>
   <sheets>
     <sheet name="_Main" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <t>Use Case #</t>
   </si>
@@ -229,9 +229,6 @@
 java -jar ./modules/apps-data-publisher/build/libs/apps-data-publisher-0.0.1-SNAPSHOT.jar --file=data/orban_putin.jpg</t>
   </si>
   <si>
-    <t>Processed image must be saved to Minio at identifier, described on 100-x-image-input</t>
-  </si>
-  <si>
     <t>frameStoragePath</t>
   </si>
   <si>
@@ -244,6 +241,30 @@
   <si>
     <t>local/jpgdata/HARON/Camera_#_0/frame_1712372019_15_382991.jpg
 local/jpgdata/HARON/C_#_/dev/github/fc/data/video.avi/frame_1712372019_15_382991.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processed image must be saved to Minio at identifier, described on 100-x-image-input
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input: jpeg image
+output: array
+[
+        {
+            "detection": 0.92,
+            "faceBox": {
+                 "p1": { "x": 507, "y": 42 },
+                 "p2": { "x": 601, "y": 165 }
+              }
+        }
+ ]
+</t>
+  </si>
+  <si>
+    <t>python FacesImageProcessor.py --file=out/orban_putin.jpg</t>
+  </si>
+  <si>
+    <t>Face recognition: input image should be processed to output result in defined format</t>
   </si>
 </sst>
 </file>
@@ -688,24 +709,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BEA9E3B-8BD1-4D8E-944C-97151E480D21}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="10"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" style="2" customWidth="1"/>
-    <col min="2" max="3" width="11.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="48.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="46.5546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="48.44140625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.77734375" style="2"/>
+    <col min="1" max="1" width="14.81640625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="11.08984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="44.36328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="48.1796875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="46.54296875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="48.453125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="10.5">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -728,16 +749,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30.6">
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="2">
         <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D2" s="3" t="s">
         <v>46</v>
       </c>
@@ -745,7 +763,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="40.799999999999997">
+    <row r="3" spans="1:7" ht="40">
       <c r="A3" s="2">
         <v>100</v>
       </c>
@@ -768,116 +786,82 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="20.399999999999999">
+    <row r="4" spans="1:7" ht="20">
       <c r="A4" s="2">
         <v>101</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D4" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="40.799999999999997">
+    <row r="5" spans="1:7" ht="40">
       <c r="A5" s="2">
         <v>102</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D5" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30.6">
+    <row r="6" spans="1:7" ht="30">
       <c r="A6" s="2">
         <v>103</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D6" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30.6">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="2">
         <v>104</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D7" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30.6">
+    <row r="8" spans="1:7" ht="30">
       <c r="A8" s="2">
         <v>105</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D8" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30.6">
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="2">
         <v>150</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D9" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30.6">
+    <row r="10" spans="1:7" ht="30">
       <c r="A10" s="2">
         <v>170</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D10" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="20.399999999999999">
+    <row r="11" spans="1:7" ht="30">
       <c r="A11" s="2">
         <v>200</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="120">
+      <c r="A12" s="2">
+        <v>300</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -936,13 +920,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="11.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="11.5"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" style="10" customWidth="1"/>
-    <col min="2" max="16384" width="8.77734375" style="10"/>
+    <col min="1" max="1" width="24.81640625" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="8.81640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="12">
+    <row r="1" spans="1:1">
       <c r="A1" s="9" t="s">
         <v>38</v>
       </c>
@@ -977,17 +961,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7EA22A1-2400-4FDB-B83E-AF4FE80BE34F}">
   <dimension ref="A2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="10"/>
   <cols>
-    <col min="1" max="1" width="29.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="33.44140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="90.21875" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="29.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.90625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="33.453125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="90.1796875" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
@@ -1022,7 +1006,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="10.5">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1102,18 +1086,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="61.2">
+    <row r="14" spans="1:4" ht="60">
       <c r="B14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+    </row>
+    <row r="16" spans="1:4" ht="10.5">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -1127,7 +1111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="234.6">
+    <row r="17" spans="2:4" ht="230">
       <c r="B17" s="6" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
UC#100: parsing cmd line parameters in java code
</commit_message>
<xml_diff>
--- a/doc/_Requrements.xlsx
+++ b/doc/_Requrements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\github\vadim-kosarev\fc\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8FA067-BEC5-4E82-948E-52CCF4F94AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286E1AB9-1F17-4259-BF8E-A1797B4EB3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="37010" windowHeight="21820" xr2:uid="{9180FCDB-912B-4427-B61B-DDCE8FA014C3}"/>
   </bookViews>
@@ -712,7 +712,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="10"/>

</xml_diff>

<commit_message>
Updated status in doc
</commit_message>
<xml_diff>
--- a/doc/_Requrements.xlsx
+++ b/doc/_Requrements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\github\vadim-kosarev\fc\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286E1AB9-1F17-4259-BF8E-A1797B4EB3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB401FDF-88F3-4976-B86E-48C6E24765BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="37010" windowHeight="21820" xr2:uid="{9180FCDB-912B-4427-B61B-DDCE8FA014C3}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="25820" windowHeight="15760" xr2:uid="{9180FCDB-912B-4427-B61B-DDCE8FA014C3}"/>
   </bookViews>
   <sheets>
     <sheet name="_Main" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="100-x-image-input" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">_Main!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">_Main!$A$1:$E$14</definedName>
+    <definedName name="Status">_ListValues!$A$1:$A$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
   <si>
     <t>Use Case #</t>
   </si>
@@ -159,31 +160,16 @@
     <t>Run example, Python</t>
   </si>
   <si>
-    <t>Run example, Java</t>
-  </si>
-  <si>
     <t>python MessagePublisher.py --file=out/orban_putin.jpg</t>
   </si>
   <si>
-    <t>Implementation Status</t>
-  </si>
-  <si>
     <t>OPEN</t>
   </si>
   <si>
     <t>IMPLEMENTED</t>
   </si>
   <si>
-    <t>Python Code</t>
-  </si>
-  <si>
-    <t>Java Code</t>
-  </si>
-  <si>
     <t>IN PROGRESS</t>
-  </si>
-  <si>
-    <t>DOC DEVELOPMENT</t>
   </si>
   <si>
     <t>UC#100 should work with Host Web Camera in Laptop  All data (timestamps, ids, frameNo-s etc…) should be calculated correctly</t>
@@ -223,10 +209,6 @@
   <si>
     <t xml:space="preserve">The system should provide prometheus data for collecting on dashboard
 </t>
-  </si>
-  <si>
-    <t>gradlew :modules:apps-data-publisher:assemble
-java -jar ./modules/apps-data-publisher/build/libs/apps-data-publisher-0.0.1-SNAPSHOT.jar --file=data/orban_putin.jpg</t>
   </si>
   <si>
     <t>frameStoragePath</t>
@@ -265,6 +247,28 @@
   </si>
   <si>
     <t>Face recognition: input image should be processed to output result in defined format</t>
+  </si>
+  <si>
+    <t>UC#100 implementation on Python</t>
+  </si>
+  <si>
+    <t>UC#100 implementation on Java</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>100.py</t>
+  </si>
+  <si>
+    <t>100.java</t>
+  </si>
+  <si>
+    <t>gradlew:assemble
+java -jar ./build/libs/jfc-app-publisher-0.0.1-SNAPSHOT.jar  --command=processImage --file=data/dflt_image.jpg</t>
   </si>
 </sst>
 </file>
@@ -321,7 +325,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,8 +338,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -343,11 +371,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -371,8 +436,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,168 +779,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BEA9E3B-8BD1-4D8E-944C-97151E480D21}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="10"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="11.08984375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="44.36328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="48.1796875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="46.54296875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="48.453125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.81640625" style="2"/>
+    <col min="1" max="1" width="14.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="44" style="2" customWidth="1"/>
+    <col min="5" max="5" width="46.5546875" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="10.5">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="30">
+    </row>
+    <row r="2" spans="1:5" ht="30.6">
       <c r="A2" s="2">
         <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="40">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30.6">
       <c r="A3" s="2">
         <v>100</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="40.799999999999997">
+      <c r="A5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20.399999999999999">
+      <c r="A6" s="2">
+        <v>101</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="3" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="40.799999999999997">
+      <c r="A7" s="2">
+        <v>102</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30.6">
+      <c r="A8" s="2">
+        <v>103</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30.6">
+      <c r="A9" s="2">
+        <v>104</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30.6">
+      <c r="A10" s="2">
+        <v>105</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30.6">
+      <c r="A11" s="2">
+        <v>150</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="3" t="s">
+    </row>
+    <row r="12" spans="1:5" ht="30.6">
+      <c r="A12" s="2">
+        <v>170</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30.6">
+      <c r="A13" s="2">
+        <v>200</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="122.4">
+      <c r="A14" s="2">
+        <v>300</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="20">
-      <c r="A4" s="2">
-        <v>101</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="40">
-      <c r="A5" s="2">
-        <v>102</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30">
-      <c r="A6" s="2">
-        <v>103</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30">
-      <c r="A7" s="2">
-        <v>104</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30">
-      <c r="A8" s="2">
-        <v>105</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30">
-      <c r="A9" s="2">
-        <v>150</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30">
-      <c r="A10" s="2">
-        <v>170</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30">
-      <c r="A11" s="2">
-        <v>200</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="120">
-      <c r="A12" s="2">
-        <v>300</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{9BEA9E3B-8BD1-4D8E-944C-97151E480D21}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G10">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="B1:C1048576">
+  <autoFilter ref="A1:E14" xr:uid="{9BEA9E3B-8BD1-4D8E-944C-97151E480D21}"/>
+  <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"OPEN"</formula>
     </cfRule>
@@ -878,14 +961,19 @@
       <formula>"IMPLEMENTED"</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{58F203D4-3CDB-4A8D-961C-977263A4F949}">
+      <formula1>Status</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{2C1A809A-DD03-4C62-B2CB-C0CBD652B8D3}">
-            <xm:f>_ListValues!$A$4</xm:f>
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{2C1A809A-DD03-4C62-B2CB-C0CBD652B8D3}">
+            <xm:f>_ListValues!$A$3</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -894,19 +982,9 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B1:C1048576</xm:sqref>
+          <xm:sqref>B1:B1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ECC11612-CB84-4B0F-A4EC-077198F2DD9A}">
-          <x14:formula1>
-            <xm:f>_ListValues!$A$2:$A$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1:C1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
     </ext>
   </extLst>
 </worksheet>
@@ -914,42 +992,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB24BA23-EDC6-405C-8413-7DDCC41366A7}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="11.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="11.4"/>
   <cols>
-    <col min="1" max="1" width="24.81640625" style="10" customWidth="1"/>
-    <col min="2" max="16384" width="8.81640625" style="10"/>
+    <col min="1" max="1" width="24.77734375" style="9" customWidth="1"/>
+    <col min="2" max="16384" width="8.77734375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="9" t="s">
-        <v>38</v>
+    <row r="1" spans="1:1" ht="12">
+      <c r="A1" s="15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="10" t="s">
-        <v>43</v>
+      <c r="A4" s="12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="A5" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="10"/>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="10"/>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="10"/>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="10"/>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -962,16 +1055,16 @@
   <dimension ref="A2:D17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="10"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999"/>
   <cols>
-    <col min="1" max="1" width="29.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.90625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="33.453125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="90.1796875" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="29.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="90.21875" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
@@ -1006,7 +1099,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="10.5">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1086,18 +1179,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="60">
+    <row r="14" spans="1:4" ht="61.2">
       <c r="B14" s="6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="10.5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -1111,7 +1204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="230">
+    <row r="17" spans="2:4" ht="234.6">
       <c r="B17" s="6" t="s">
         <v>28</v>
       </c>

</xml_diff>